<commit_message>
Apply current date as assigned by end user
</commit_message>
<xml_diff>
--- a/adg-api/src/main/resources/bidv/bang-ke-su-dung-tien-vay.xlsx
+++ b/adg-api/src/main/resources/bidv/bang-ke-su-dung-tien-vay.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services/adg-server/src/main/resources/bidv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luan.phm/engineering/Projects/ADongGroup/adg-services-v2/adg-api/src/main/resources/bidv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBA0C07-09F4-1146-A915-4DE8ECC5A947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68931DC3-35DE-1047-975C-E67EA959FCF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,32 +39,6 @@
     <t>BẢNG KÊ SỬ DỤNG TIỀN VAY</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="&quot;Times New Roman&quot;, serif"/>
-      </rPr>
-      <t xml:space="preserve">Chi tiết nội dung sử dụng tiền vay theo hợp đồng tín dụng ngắn hạn cụ thể số : 01.219/2021/8088928/HĐTD ngày </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="&quot;Times New Roman&quot;, serif"/>
-      </rPr>
-      <t>{{current_date}}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="&quot;Times New Roman&quot;, serif"/>
-      </rPr>
-      <t xml:space="preserve"> được ký kết giữa Ngân hàng và Bên vay.</t>
-    </r>
-  </si>
-  <si>
     <t>TT</t>
   </si>
   <si>
@@ -85,6 +59,12 @@
   </si>
   <si>
     <t>Tổng cộng</t>
+  </si>
+  <si>
+    <t>BÊN VAY</t>
+  </si>
+  <si>
+    <t>Chi tiết nội dung sử dụng tiền vay theo hợp đồng tín dụng ngắn hạn cụ thể số : 01.219/2021/8088928/HĐTD ngày 15/06/2021 được ký kết giữa Ngân hàng và Bên vay.</t>
   </si>
   <si>
     <r>
@@ -101,7 +81,7 @@
         <color rgb="FFFF0000"/>
         <rFont val="&quot;Times New Roman&quot;, serif"/>
       </rPr>
-      <t>{{current_date}}</t>
+      <t>15/06/2021</t>
     </r>
     <r>
       <rPr>
@@ -111,9 +91,6 @@
       </rPr>
       <t xml:space="preserve"> được ký kết giữa Ngân hàng và Bên vay.</t>
     </r>
-  </si>
-  <si>
-    <t>BÊN VAY</t>
   </si>
 </sst>
 </file>
@@ -300,8 +277,8 @@
     <xf numFmtId="3" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -317,8 +294,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,9 +517,7 @@
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -608,8 +583,8 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="14">
-      <c r="A7" s="17" t="s">
-        <v>3</v>
+      <c r="A7" s="24" t="s">
+        <v>11</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
@@ -627,22 +602,22 @@
     </row>
     <row r="9" spans="1:6" ht="39.75" customHeight="1">
       <c r="A9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15">
@@ -655,11 +630,11 @@
     </row>
     <row r="11" spans="1:6" ht="15">
       <c r="A11" s="22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
@@ -672,8 +647,8 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:6" ht="14">
-      <c r="A13" s="17" t="s">
-        <v>11</v>
+      <c r="A13" s="24" t="s">
+        <v>12</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -690,7 +665,7 @@
     </row>
     <row r="15" spans="1:6" ht="15">
       <c r="F15" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>